<commit_message>
add ISD1820 documentation etc
</commit_message>
<xml_diff>
--- a/files/components.xlsx
+++ b/files/components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ralphroossen/Github-repos/ageofdust/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA0EA20-41B9-084B-8D7E-78DE22B752CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5BE273-9B07-644D-8C1F-DA76B920E289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="17000" xr2:uid="{F1C1B904-D015-A44E-AAE6-E5F7FD6E4450}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="87">
   <si>
     <t>order nr</t>
   </si>
@@ -59,18 +59,12 @@
     <t>Hall effect switch module</t>
   </si>
   <si>
-    <t>NE555 Pulse generator module</t>
-  </si>
-  <si>
     <t>Piezo w soldered wires 35 mm</t>
   </si>
   <si>
     <t>Vibration sensor module 3-5V</t>
   </si>
   <si>
-    <t>Rain sensor</t>
-  </si>
-  <si>
     <t xml:space="preserve">Light sensormodule </t>
   </si>
   <si>
@@ -92,18 +86,12 @@
     <t>000769</t>
   </si>
   <si>
-    <t>001337</t>
-  </si>
-  <si>
     <t>000887</t>
   </si>
   <si>
     <t>000752</t>
   </si>
   <si>
-    <t>000372</t>
-  </si>
-  <si>
     <t>000208</t>
   </si>
   <si>
@@ -149,24 +137,12 @@
     <t>https://www.tinytronics.nl/shop/en/sensors/magnetic-field/hall-effect-switch-module</t>
   </si>
   <si>
-    <t>https://www.tinytronics.nl/shop/en/communication-and-signals/signal-generators-and-dacs/ne555-frequency-adjustable-pulse-generator</t>
-  </si>
-  <si>
-    <t>5-12V</t>
-  </si>
-  <si>
     <t>https://www.tinytronics.nl/shop/en/audio/speakers/buzzers/piezo-electronic-buzzer-with-soldered-wires-35mm</t>
   </si>
   <si>
     <t>https://www.tinytronics.nl/shop/en/sensors/acceleration-rotation/vibration-sensor-module-3-5v-sw-18010p</t>
   </si>
   <si>
-    <t>3.3-5V</t>
-  </si>
-  <si>
-    <t>https://www.tinytronics.nl/shop/en/sensors/liquid/rain-sensor</t>
-  </si>
-  <si>
     <t>https://www.tinytronics.nl/shop/en/sensors/optical/light-and-color/red-laser-sensor-module</t>
   </si>
   <si>
@@ -278,13 +254,46 @@
     <t>https://www.lidl.nl/p/silvercrest-walkie-talkies-voor-kinderen/p100359077002?mktc=shopping</t>
   </si>
   <si>
-    <t>6 x AAA (LR03)</t>
-  </si>
-  <si>
     <t xml:space="preserve">12x AAA (LR02 Batteries) </t>
   </si>
   <si>
     <t>Postage Lidl</t>
+  </si>
+  <si>
+    <t>4.5V (3 x AAA per walkie)</t>
+  </si>
+  <si>
+    <t>8 ohm speaker</t>
+  </si>
+  <si>
+    <t>Jack connector 3.5 solderable</t>
+  </si>
+  <si>
+    <t>jumpers MM</t>
+  </si>
+  <si>
+    <t>jumpers FF</t>
+  </si>
+  <si>
+    <t>jumpers MF</t>
+  </si>
+  <si>
+    <t>solid core hookup wire</t>
+  </si>
+  <si>
+    <t>shrinktube</t>
+  </si>
+  <si>
+    <t>stranded hookup wire</t>
+  </si>
+  <si>
+    <t>500K pot (or 250K!)</t>
+  </si>
+  <si>
+    <t>conductive materials</t>
+  </si>
+  <si>
+    <t>some regular switches</t>
   </si>
 </sst>
 </file>
@@ -736,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0861264C-AD37-A740-8F85-E647F2523065}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -758,19 +767,19 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>0</v>
@@ -781,7 +790,7 @@
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D2" s="17"/>
       <c r="E2" s="11"/>
@@ -790,13 +799,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E4" s="12">
         <v>2.5</v>
@@ -806,10 +815,10 @@
         <v>0</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -826,14 +835,14 @@
         <v>2</v>
       </c>
       <c r="F5" s="12">
-        <f t="shared" ref="F5:F23" si="0">D5*E5</f>
+        <f t="shared" ref="F5:F21" si="0">D5*E5</f>
         <v>4</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -841,7 +850,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D6" s="17">
         <v>5</v>
@@ -854,15 +863,15 @@
         <v>37.5</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12">
@@ -872,10 +881,10 @@
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="13">
@@ -886,15 +895,15 @@
         <v>0</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="13">
@@ -905,10 +914,10 @@
         <v>0</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -916,7 +925,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D10" s="17">
         <v>2</v>
@@ -929,60 +938,60 @@
         <v>3</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="H10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>39</v>
-      </c>
+      <c r="B11" s="7"/>
       <c r="D11" s="17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E11" s="12">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="F11" s="12">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="7"/>
+      <c r="B12" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="D12" s="17">
+        <v>2</v>
+      </c>
+      <c r="E12" s="12">
+        <v>2</v>
+      </c>
+      <c r="F12" s="12">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E12" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="F12" s="12">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
       <c r="G12" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H12" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="7" t="s">
@@ -992,168 +1001,168 @@
         <v>2</v>
       </c>
       <c r="E13" s="12">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="F13" s="12">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="D14" s="17">
         <v>2</v>
       </c>
       <c r="E14" s="12">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="F14" s="12">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="17">
+      <c r="B15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="20">
         <v>2</v>
       </c>
-      <c r="E15" s="12">
-        <v>2.5</v>
+      <c r="E15" s="14">
+        <v>4</v>
       </c>
       <c r="F15" s="12">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" t="s">
-        <v>34</v>
+        <v>8</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>16</v>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
       </c>
       <c r="D16" s="17">
         <v>2</v>
       </c>
       <c r="E16" s="12">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="F16" s="12">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="20">
-        <v>2</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="D17" s="20"/>
       <c r="E17" s="14">
-        <v>4</v>
+        <v>0.75</v>
       </c>
       <c r="F17" s="12">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>45</v>
+        <v>0</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H17" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" t="s">
         <v>48</v>
       </c>
       <c r="D18" s="17">
         <v>2</v>
       </c>
       <c r="E18" s="12">
-        <v>1.5</v>
+        <v>5</v>
       </c>
       <c r="F18" s="12">
         <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="20">
+        <v>10</v>
+      </c>
+      <c r="E19" s="14">
         <v>3</v>
       </c>
-      <c r="G18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="14">
-        <v>0.75</v>
-      </c>
       <c r="F19" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="H19" t="s">
-        <v>49</v>
+        <v>30</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1161,148 +1170,201 @@
         <v>55</v>
       </c>
       <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="17">
+        <v>10</v>
+      </c>
+      <c r="E20" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="F20" s="12">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="17">
+      <c r="H20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="17">
         <v>2</v>
       </c>
-      <c r="E20" s="12">
-        <v>5</v>
-      </c>
-      <c r="F20" s="12">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="20">
-        <v>10</v>
-      </c>
-      <c r="E21" s="14">
-        <v>3</v>
+      <c r="E21" s="12">
+        <v>29.99</v>
       </c>
       <c r="F21" s="12">
         <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B22" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="17">
-        <v>10</v>
-      </c>
-      <c r="E22" s="12">
-        <v>3.5</v>
-      </c>
-      <c r="F22" s="12">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="H22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B23" t="s">
+        <v>59.98</v>
+      </c>
+      <c r="H21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="19"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="19"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="19"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="8"/>
+    </row>
+    <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" s="19"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" s="19"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="8"/>
+    </row>
+    <row r="27" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="19"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="8"/>
+    </row>
+    <row r="28" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D23" s="17">
-        <v>2</v>
-      </c>
-      <c r="E23" s="12">
-        <v>29.99</v>
-      </c>
-      <c r="F23" s="12">
-        <f t="shared" si="0"/>
-        <v>59.98</v>
-      </c>
-      <c r="H23" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
+      <c r="D28" s="19"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="8"/>
+    </row>
+    <row r="29" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" s="19"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-    </row>
-    <row r="26" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="21"/>
-      <c r="E26" s="15">
+      <c r="D30" s="19"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="8"/>
+    </row>
+    <row r="31" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" s="19"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="8"/>
+    </row>
+    <row r="32" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="19"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="8"/>
+    </row>
+    <row r="33" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33" s="19"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="8"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+    </row>
+    <row r="35" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="21"/>
+      <c r="E35" s="15">
         <v>2.5</v>
       </c>
-      <c r="F26" s="15"/>
-      <c r="G26" s="6"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E27" s="15">
+      <c r="F35" s="15"/>
+      <c r="G35" s="6"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E36" s="15">
         <v>4.99</v>
       </c>
-      <c r="F27" s="15"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="5"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="5"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C30" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="5"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="5"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C39" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="11"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="G8:G11 G4 G5:G6 G12:G22" numberStoredAsText="1"/>
+    <ignoredError sqref="G8:G10 G4 G5:G6 G11:G12 G13:G20" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>